<commit_message>
working on assignment3 report.
</commit_message>
<xml_diff>
--- a/Assignment3/report/Assignment_3-plot_Kazumi.xlsx
+++ b/Assignment3/report/Assignment_3-plot_Kazumi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KAZUMI\repo\cse436\Assignment3\Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KAZUMI\repo\cse436\Assignment3\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -474,11 +474,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115151448"/>
-        <c:axId val="115147920"/>
+        <c:axId val="124890584"/>
+        <c:axId val="124891368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115151448"/>
+        <c:axId val="124890584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -511,7 +511,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115147920"/>
+        <c:crossAx val="124891368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -519,7 +519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115147920"/>
+        <c:axId val="124891368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +549,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115151448"/>
+        <c:crossAx val="124890584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -798,11 +798,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="115145960"/>
-        <c:axId val="115152232"/>
+        <c:axId val="124892544"/>
+        <c:axId val="124892936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="115145960"/>
+        <c:axId val="124892544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -831,7 +831,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115152232"/>
+        <c:crossAx val="124892936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -839,7 +839,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115152232"/>
+        <c:axId val="124892936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +874,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115145960"/>
+        <c:crossAx val="124892544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1302,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C21:H41"/>
+  <dimension ref="C21:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1388,6 +1388,10 @@
       <c r="G26">
         <v>203.99999600000001</v>
       </c>
+      <c r="H26">
+        <f>G26/G27</f>
+        <v>2.2173910680529509</v>
+      </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
@@ -1424,25 +1428,55 @@
       </c>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="D29" s="3">
+        <f>D26/D27</f>
+        <v>0.99976203950144271</v>
+      </c>
+      <c r="E29" s="3">
+        <f t="shared" ref="E29:G29" si="0">E26/E27</f>
+        <v>1.2499849373079508</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9333535379582723</v>
+      </c>
+      <c r="G29" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2173910680529509</v>
+      </c>
+      <c r="H29" s="1">
+        <f>G27/G28</f>
+        <v>3.5384587159788281</v>
+      </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="D30" s="2">
+        <f>D26/D28</f>
+        <v>0.50000025001812631</v>
+      </c>
+      <c r="E30" s="2">
+        <f>E26/E28</f>
+        <v>2.4998217582882396</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" ref="E30:G30" si="1">F26/F28</f>
+        <v>4.8333068335188321</v>
+      </c>
+      <c r="G30" s="2">
+        <f>G26/G28</f>
+        <v>7.8461467514855672</v>
+      </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="1">
+        <f>G25/G28</f>
+        <v>105.4229812412089</v>
+      </c>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D32" s="2"/>
@@ -1530,6 +1564,66 @@
       </c>
       <c r="G41" s="5">
         <v>24.999856999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E43">
+        <f>E39/E40</f>
+        <v>2.4780110935023769</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E44">
+        <f>E39/E41</f>
+        <v>24.245380540121463</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <f>E40/E41</f>
+        <v>9.7842098462333631</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <f>D39/G39</f>
+        <v>5.2090626268151113E-2</v>
+      </c>
+      <c r="E47">
+        <f>E39/G39</f>
+        <v>0.91977835221611381</v>
+      </c>
+      <c r="F47">
+        <f>F39/G39</f>
+        <v>2.9649475648888344E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <f t="shared" ref="D48:D49" si="2">D40/G40</f>
+        <v>0.11456459620106188</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ref="E48:E49" si="3">E40/G40</f>
+        <v>0.81419411744750148</v>
+      </c>
+      <c r="F48">
+        <f t="shared" ref="F48:F49" si="4">F40/G40</f>
+        <v>6.521509934388664E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>0.42504243124270669</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="3"/>
+        <v>0.30956177069332835</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="4"/>
+        <v>0.23832136319819752</v>
       </c>
     </row>
   </sheetData>

</xml_diff>